<commit_message>
meta py und rearrangement anpassung ans modell
meta py und rearrangement an nvto.tll änderungen angepasst
</commit_message>
<xml_diff>
--- a/Mapping_Meta_Py.xlsx
+++ b/Mapping_Meta_Py.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Dropbox\ITI\Projektmodul\nvtxlsxrdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53651F66-1EF7-4029-AD91-A8778C24BDFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C5A1A7-078B-423F-8135-E891C2114D97}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="927" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produktionen" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="466">
   <si>
     <t>Identifier / geeinigter Name</t>
   </si>
@@ -849,9 +849,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>nvto:occuredAtTime</t>
-  </si>
-  <si>
     <t>occured at time</t>
   </si>
   <si>
@@ -936,9 +933,6 @@
     <t>Date Created</t>
   </si>
   <si>
-    <t>nvto:originatedAtPlace</t>
-  </si>
-  <si>
     <t>originated at place</t>
   </si>
   <si>
@@ -1393,6 +1387,57 @@
   </si>
   <si>
     <t>texts2</t>
+  </si>
+  <si>
+    <t>season1</t>
+  </si>
+  <si>
+    <t>season2</t>
+  </si>
+  <si>
+    <t>referenziert Produktion</t>
+  </si>
+  <si>
+    <t>beruht auf Produktion</t>
+  </si>
+  <si>
+    <t>Wiederaufnahme von</t>
+  </si>
+  <si>
+    <t>Erstaufführungsversion von</t>
+  </si>
+  <si>
+    <t>Nachfolger von</t>
+  </si>
+  <si>
+    <t>weitere Typen</t>
+  </si>
+  <si>
+    <t>nvto:isRestagedVersionOf</t>
+  </si>
+  <si>
+    <t>nvto:isFirstPerformanceVersionOf</t>
+  </si>
+  <si>
+    <t>is influenced by</t>
+  </si>
+  <si>
+    <t>has  predecessor</t>
+  </si>
+  <si>
+    <t>is restaged version of</t>
+  </si>
+  <si>
+    <t>is first performance version of</t>
+  </si>
+  <si>
+    <t>nvto:PROPOSED_isInfluencedBy</t>
+  </si>
+  <si>
+    <t>nvto:hasTimeOfOccurence</t>
+  </si>
+  <si>
+    <t>nvto:hasPlaceOfOrigin</t>
   </si>
 </sst>
 </file>
@@ -1955,20 +2000,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="9" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" style="9" customWidth="1"/>
     <col min="8" max="8" width="37" style="9" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="9"/>
@@ -1985,7 +2030,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -1994,10 +2039,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2011,7 +2056,7 @@
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
       <c r="G2" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H2" s="25"/>
     </row>
@@ -2022,27 +2067,28 @@
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="E3" s="26" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>198</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H3" s="25"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>445</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
-      <c r="G4" s="28" t="s">
-        <v>447</v>
-      </c>
+      <c r="G4" s="28"/>
       <c r="H4" s="28"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -2050,14 +2096,15 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>446</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
-      <c r="G5" s="28" t="s">
-        <v>448</v>
-      </c>
+      <c r="G5" s="28"/>
       <c r="H5" s="28"/>
       <c r="I5"/>
       <c r="J5"/>
@@ -2065,31 +2112,33 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>447</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
-      <c r="G6" s="25" t="s">
-        <v>449</v>
-      </c>
+      <c r="G6" s="25"/>
       <c r="H6" s="25" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>448</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="25" t="s">
-        <v>450</v>
-      </c>
+      <c r="G7" s="25"/>
       <c r="H7" s="25" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2098,558 +2147,639 @@
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>201</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
+        <v>451</v>
+      </c>
       <c r="E9" s="26" t="s">
-        <v>391</v>
+        <v>263</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>202</v>
+        <v>264</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H9" s="25"/>
+        <v>444</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+        <v>452</v>
+      </c>
       <c r="E10" s="26" t="s">
-        <v>203</v>
+        <v>463</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>204</v>
+        <v>459</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H10" s="25"/>
+        <v>444</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
+        <v>453</v>
+      </c>
       <c r="E11" s="26" t="s">
-        <v>205</v>
+        <v>457</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>206</v>
+        <v>461</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H11" s="25"/>
+        <v>444</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+        <v>454</v>
+      </c>
       <c r="E12" s="26" t="s">
-        <v>207</v>
+        <v>458</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>208</v>
+        <v>462</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H12" s="25"/>
+        <v>444</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+        <v>455</v>
+      </c>
       <c r="E13" s="26" t="s">
-        <v>209</v>
+        <v>362</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>210</v>
+        <v>460</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H13" s="25"/>
+        <v>444</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H14" s="25"/>
+        <v>456</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="26" t="s">
-        <v>213</v>
+        <v>389</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="26" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
       <c r="E17" s="26" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="26" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="26" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="26" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="26" t="s">
-        <v>443</v>
+        <v>213</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="26" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H22" s="25"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
       <c r="E23" s="26" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="26" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H24" s="25"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
       <c r="E25" s="26" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="26" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H26" s="25"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="26" t="s">
-        <v>235</v>
+        <v>441</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H27" s="25"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
-      <c r="E28" s="25" t="s">
-        <v>417</v>
-      </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25" t="s">
-        <v>418</v>
-      </c>
+      <c r="E28" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>444</v>
+      </c>
+      <c r="H28" s="25"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
       <c r="E29" s="26" t="s">
-        <v>391</v>
+        <v>227</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H29" s="25"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="26" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H30" s="25"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="26" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H31" s="25"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>249</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="26" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H32" s="25"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>249</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C33" s="24"/>
       <c r="D33" s="24"/>
       <c r="E33" s="26" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H33" s="25"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
-      <c r="E34" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H34" s="25"/>
+      <c r="E34" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="26" t="s">
-        <v>247</v>
+        <v>389</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>248</v>
+        <v>202</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H35" s="25"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>443</v>
+      </c>
+      <c r="H36" s="25"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>443</v>
+      </c>
+      <c r="H37" s="25"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>443</v>
+      </c>
+      <c r="H38" s="25"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D39" s="24"/>
+      <c r="E39" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>443</v>
+      </c>
+      <c r="H39" s="25"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="F36" s="27" t="s">
+      <c r="F40" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="G36" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H36" s="25"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="G40" s="25" t="s">
+        <v>444</v>
+      </c>
+      <c r="H40" s="25"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>444</v>
+      </c>
+      <c r="H41" s="25"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>444</v>
+      </c>
+      <c r="H42" s="25"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B43" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="24" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E43" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F43" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="G37" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="H37" s="25"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="G43" s="25" t="s">
+        <v>444</v>
+      </c>
+      <c r="H43" s="25"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="26" t="s">
-        <v>392</v>
-      </c>
-      <c r="F38" s="27" t="s">
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="F44" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="G38" s="25" t="s">
-        <v>445</v>
-      </c>
-      <c r="H38" s="25"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="G44" s="25" t="s">
+        <v>443</v>
+      </c>
+      <c r="H44" s="25"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="F39" s="27" t="s">
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="F45" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="G39" s="25" t="s">
-        <v>445</v>
-      </c>
-      <c r="H39" s="25"/>
+      <c r="G45" s="25" t="s">
+        <v>443</v>
+      </c>
+      <c r="H45" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2686,7 +2816,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -2695,10 +2825,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2706,7 +2836,7 @@
         <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2714,13 +2844,13 @@
         <v>185</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>260</v>
       </c>
       <c r="G3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H3" s="18"/>
     </row>
@@ -2731,7 +2861,7 @@
       <c r="E4" s="22"/>
       <c r="F4" s="3"/>
       <c r="H4" s="18" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2739,13 +2869,13 @@
         <v>187</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H5" s="18"/>
     </row>
@@ -2754,7 +2884,7 @@
         <v>188</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>262</v>
@@ -2765,10 +2895,10 @@
         <v>180</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2776,10 +2906,10 @@
         <v>181</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2787,10 +2917,10 @@
         <v>183</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -2828,7 +2958,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -2837,10 +2967,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2848,7 +2978,7 @@
         <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2856,13 +2986,13 @@
         <v>190</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>260</v>
       </c>
       <c r="G3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H3" s="18"/>
     </row>
@@ -2873,7 +3003,7 @@
       <c r="E4" s="22"/>
       <c r="F4" s="3"/>
       <c r="H4" s="18" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2881,13 +3011,13 @@
         <v>192</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H5" s="18"/>
     </row>
@@ -2896,10 +3026,10 @@
         <v>180</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2907,10 +3037,10 @@
         <v>181</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2918,10 +3048,10 @@
         <v>183</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2963,7 +3093,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -2972,7 +3102,7 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2980,7 +3110,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2988,10 +3118,10 @@
         <v>193</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H3" s="18"/>
     </row>
@@ -3010,7 +3140,7 @@
         <v>251</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>199</v>
@@ -3048,7 +3178,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -3057,7 +3187,7 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3065,7 +3195,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3073,10 +3203,10 @@
         <v>196</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H3" s="18"/>
     </row>
@@ -3097,7 +3227,7 @@
         <v>251</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>199</v>
@@ -3113,7 +3243,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,7 +3269,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -3148,10 +3278,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3159,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3167,7 +3297,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>260</v>
@@ -3178,7 +3308,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>201</v>
@@ -3199,7 +3329,7 @@
         <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>262</v>
@@ -3232,7 +3362,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>262</v>
@@ -3243,7 +3373,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>202</v>
@@ -3375,7 +3505,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>225</v>
@@ -3452,7 +3582,7 @@
         <v>41</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>265</v>
@@ -3474,7 +3604,7 @@
         <v>27</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>202</v>
@@ -3485,12 +3615,12 @@
         <v>26</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3498,7 +3628,7 @@
         <v>43</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>268</v>
@@ -3509,7 +3639,7 @@
         <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>243</v>
@@ -3523,7 +3653,7 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>245</v>
@@ -3537,10 +3667,10 @@
         <v>32</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3548,10 +3678,10 @@
         <v>33</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3559,10 +3689,10 @@
         <v>34</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3573,7 +3703,7 @@
         <v>259</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>261</v>
@@ -3581,19 +3711,19 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B41" t="s">
         <v>259</v>
       </c>
       <c r="D41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3605,8 +3735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,7 +3762,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -3641,10 +3771,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3652,10 +3782,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3663,12 +3793,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3676,7 +3806,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3684,10 +3814,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3695,10 +3825,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3706,10 +3836,10 @@
         <v>51</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3717,10 +3847,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3728,13 +3858,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3742,7 +3872,7 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>262</v>
@@ -3753,7 +3883,7 @@
         <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>262</v>
@@ -3764,7 +3894,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>262</v>
@@ -3775,10 +3905,10 @@
         <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3786,10 +3916,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3808,10 +3938,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3830,7 +3960,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -3841,10 +3971,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3862,10 +3992,10 @@
         <v>66</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>284</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3873,10 +4003,10 @@
         <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3884,10 +4014,10 @@
         <v>68</v>
       </c>
       <c r="E24" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3917,10 +4047,10 @@
         <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4005,7 +4135,7 @@
         <v>19</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>225</v>
@@ -4093,7 +4223,7 @@
         <v>27</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>202</v>
@@ -4104,10 +4234,10 @@
         <v>74</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -4115,10 +4245,10 @@
         <v>75</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -4126,12 +4256,12 @@
         <v>26</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4139,10 +4269,10 @@
         <v>76</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4150,10 +4280,10 @@
         <v>77</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -4161,10 +4291,10 @@
         <v>78</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -4172,10 +4302,10 @@
         <v>33</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -4183,10 +4313,10 @@
         <v>34</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -4194,13 +4324,13 @@
         <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -4208,13 +4338,13 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -4237,13 +4367,13 @@
         <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E57" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F57" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -4251,13 +4381,13 @@
         <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -4265,10 +4395,10 @@
         <v>86</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4276,7 +4406,7 @@
         <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E60" s="9"/>
     </row>
@@ -4292,7 +4422,7 @@
         <v>89</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F62" s="3"/>
     </row>
@@ -4301,13 +4431,13 @@
         <v>90</v>
       </c>
       <c r="C63" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -4315,13 +4445,13 @@
         <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -4329,13 +4459,13 @@
         <v>92</v>
       </c>
       <c r="C65" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4343,13 +4473,13 @@
         <v>93</v>
       </c>
       <c r="C66" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4357,10 +4487,10 @@
         <v>94</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4371,7 +4501,7 @@
         <v>259</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>199</v>
@@ -4379,47 +4509,47 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B69" t="s">
         <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B70" t="s">
         <v>259</v>
       </c>
       <c r="D70" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B71" t="s">
         <v>259</v>
       </c>
       <c r="D71" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -4458,7 +4588,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -4467,10 +4597,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4478,10 +4608,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4489,12 +4619,12 @@
         <v>95</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4502,7 +4632,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4510,10 +4640,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4521,10 +4651,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4532,10 +4662,10 @@
         <v>96</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4543,10 +4673,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4554,13 +4684,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4568,7 +4698,7 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>262</v>
@@ -4579,7 +4709,7 @@
         <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>262</v>
@@ -4590,7 +4720,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>262</v>
@@ -4601,10 +4731,10 @@
         <v>98</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4612,10 +4742,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4623,10 +4753,10 @@
         <v>59</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4634,10 +4764,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4645,10 +4775,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4656,7 +4786,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -4667,10 +4797,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4688,10 +4818,10 @@
         <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4699,10 +4829,10 @@
         <v>100</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4710,10 +4840,10 @@
         <v>101</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4721,10 +4851,10 @@
         <v>102</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4743,10 +4873,10 @@
         <v>104</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4754,10 +4884,10 @@
         <v>105</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4765,10 +4895,10 @@
         <v>106</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4776,10 +4906,10 @@
         <v>107</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4787,7 +4917,7 @@
         <v>27</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>202</v>
@@ -4798,10 +4928,10 @@
         <v>108</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -4809,10 +4939,10 @@
         <v>109</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -4820,7 +4950,7 @@
         <v>110</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -4829,7 +4959,7 @@
         <v>111</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -4838,10 +4968,10 @@
         <v>112</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -4849,10 +4979,10 @@
         <v>113</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4860,10 +4990,10 @@
         <v>114</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -4871,10 +5001,10 @@
         <v>115</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -4882,10 +5012,10 @@
         <v>116</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -4893,10 +5023,10 @@
         <v>117</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -4904,10 +5034,10 @@
         <v>34</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -4915,7 +5045,7 @@
         <v>118</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>201</v>
@@ -4926,7 +5056,7 @@
         <v>119</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>200</v>
@@ -4937,10 +5067,10 @@
         <v>120</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -4948,13 +5078,13 @@
         <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4962,13 +5092,13 @@
         <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4976,10 +5106,10 @@
         <v>121</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -4994,13 +5124,13 @@
         <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5028,7 +5158,7 @@
         <v>89</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F54" s="3"/>
     </row>
@@ -5037,13 +5167,13 @@
         <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -5051,13 +5181,13 @@
         <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -5065,13 +5195,13 @@
         <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -5079,10 +5209,10 @@
         <v>94</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -5093,7 +5223,7 @@
         <v>259</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>199</v>
@@ -5101,47 +5231,47 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B60" t="s">
         <v>259</v>
       </c>
       <c r="C60" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B61" t="s">
         <v>259</v>
       </c>
       <c r="D61" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B62" t="s">
         <v>259</v>
       </c>
       <c r="D62" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -5181,7 +5311,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -5190,10 +5320,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5201,10 +5331,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5212,12 +5342,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5225,7 +5355,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5233,10 +5363,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5244,16 +5374,16 @@
         <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5261,10 +5391,10 @@
         <v>50</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5272,10 +5402,10 @@
         <v>51</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5283,10 +5413,10 @@
         <v>52</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5294,13 +5424,13 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5308,7 +5438,7 @@
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>262</v>
@@ -5319,7 +5449,7 @@
         <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>262</v>
@@ -5330,7 +5460,7 @@
         <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>262</v>
@@ -5341,10 +5471,10 @@
         <v>126</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5352,10 +5482,10 @@
         <v>58</v>
       </c>
       <c r="E15" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5363,10 +5493,10 @@
         <v>59</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -5375,10 +5505,10 @@
         <v>60</v>
       </c>
       <c r="E17" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5386,10 +5516,10 @@
         <v>61</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -5397,7 +5527,7 @@
         <v>127</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>198</v>
@@ -5418,10 +5548,10 @@
         <v>129</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -5429,10 +5559,10 @@
         <v>130</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5440,10 +5570,10 @@
         <v>131</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5451,10 +5581,10 @@
         <v>132</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5462,10 +5592,10 @@
         <v>133</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -5473,10 +5603,10 @@
         <v>134</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -5484,10 +5614,10 @@
         <v>135</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5495,13 +5625,13 @@
         <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5509,13 +5639,13 @@
         <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5523,10 +5653,10 @@
         <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>199</v>
@@ -5537,13 +5667,13 @@
         <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5551,10 +5681,10 @@
         <v>86</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5562,10 +5692,10 @@
         <v>121</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -5573,13 +5703,13 @@
         <v>139</v>
       </c>
       <c r="C35" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -5587,10 +5717,10 @@
         <v>140</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -5598,13 +5728,13 @@
         <v>141</v>
       </c>
       <c r="C37" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -5625,7 +5755,7 @@
         <v>89</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -5634,13 +5764,13 @@
         <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -5648,13 +5778,13 @@
         <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -5662,13 +5792,13 @@
         <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -5676,12 +5806,12 @@
         <v>94</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
       <c r="H44" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -5692,7 +5822,7 @@
         <v>259</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>199</v>
@@ -5700,47 +5830,47 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B46" t="s">
         <v>259</v>
       </c>
       <c r="C46" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B47" t="s">
         <v>259</v>
       </c>
       <c r="D47" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B48" t="s">
         <v>259</v>
       </c>
       <c r="D48" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -5779,7 +5909,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -5788,10 +5918,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5799,10 +5929,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5810,12 +5940,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5823,7 +5953,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5831,10 +5961,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5842,10 +5972,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5853,10 +5983,10 @@
         <v>51</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5864,10 +5994,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5875,13 +6005,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5889,7 +6019,7 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>262</v>
@@ -5900,7 +6030,7 @@
         <v>142</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>262</v>
@@ -5911,7 +6041,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>262</v>
@@ -5922,10 +6052,10 @@
         <v>143</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5933,10 +6063,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5947,7 +6077,7 @@
         <v>263</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5955,10 +6085,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5969,7 +6099,7 @@
         <v>263</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5977,7 +6107,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -5988,10 +6118,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -6009,10 +6139,10 @@
         <v>68</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6023,7 +6153,7 @@
         <v>263</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -6031,10 +6161,10 @@
         <v>144</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -6056,7 +6186,7 @@
         <v>263</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -6064,12 +6194,12 @@
         <v>26</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -6077,10 +6207,10 @@
         <v>76</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -6088,10 +6218,10 @@
         <v>77</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -6099,10 +6229,10 @@
         <v>78</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -6110,10 +6240,10 @@
         <v>33</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -6121,10 +6251,10 @@
         <v>34</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -6132,13 +6262,13 @@
         <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -6146,13 +6276,13 @@
         <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -6176,16 +6306,16 @@
         <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H38" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -6193,10 +6323,10 @@
         <v>86</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -6217,7 +6347,7 @@
         <v>89</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -6226,13 +6356,13 @@
         <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -6240,13 +6370,13 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -6254,13 +6384,13 @@
         <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -6268,13 +6398,13 @@
         <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -6282,12 +6412,12 @@
         <v>94</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
       <c r="H47" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -6298,7 +6428,7 @@
         <v>259</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>199</v>
@@ -6306,47 +6436,47 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B49" t="s">
         <v>259</v>
       </c>
       <c r="C49" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B50" t="s">
         <v>259</v>
       </c>
       <c r="D50" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B51" t="s">
         <v>259</v>
       </c>
       <c r="D51" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -6384,7 +6514,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -6393,10 +6523,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6404,7 +6534,7 @@
         <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6412,10 +6542,10 @@
         <v>148</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6423,10 +6553,10 @@
         <v>149</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6434,10 +6564,10 @@
         <v>150</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6455,10 +6585,10 @@
         <v>151</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6466,10 +6596,10 @@
         <v>152</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6477,13 +6607,13 @@
         <v>153</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6491,10 +6621,10 @@
         <v>154</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6502,10 +6632,10 @@
         <v>155</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6513,10 +6643,10 @@
         <v>156</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6524,10 +6654,10 @@
         <v>157</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6535,10 +6665,10 @@
         <v>158</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6546,10 +6676,10 @@
         <v>159</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -6560,7 +6690,7 @@
         <v>259</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>261</v>
@@ -6602,7 +6732,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -6611,10 +6741,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6622,7 +6752,7 @@
         <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6630,7 +6760,7 @@
         <v>161</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>260</v>
@@ -6641,10 +6771,10 @@
         <v>162</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6670,10 +6800,10 @@
         <v>164</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6681,10 +6811,10 @@
         <v>165</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6714,10 +6844,10 @@
         <v>168</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6725,10 +6855,10 @@
         <v>157</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6736,10 +6866,10 @@
         <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6747,10 +6877,10 @@
         <v>170</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6766,7 +6896,7 @@
         <v>259</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>199</v>
@@ -6808,7 +6938,7 @@
         <v>257</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>253</v>
@@ -6817,10 +6947,10 @@
         <v>254</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6828,7 +6958,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6843,7 +6973,7 @@
         <v>174</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>260</v>
@@ -6855,10 +6985,10 @@
         <v>175</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6888,10 +7018,10 @@
         <v>176</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -6899,7 +7029,7 @@
         <v>177</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>262</v>
@@ -6910,7 +7040,7 @@
         <v>178</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>262</v>
@@ -6921,7 +7051,7 @@
         <v>179</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>262</v>
@@ -6932,10 +7062,10 @@
         <v>180</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -6943,10 +7073,10 @@
         <v>181</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6954,10 +7084,10 @@
         <v>182</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -6965,10 +7095,10 @@
         <v>170</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -6976,10 +7106,10 @@
         <v>169</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -6987,10 +7117,10 @@
         <v>183</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -7001,7 +7131,7 @@
         <v>259</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>199</v>
@@ -7009,19 +7139,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B19" t="s">
         <v>259</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>